<commit_message>
Dossier : avancées sur le corpus
</commit_message>
<xml_diff>
--- a/dossiers/stats_corpus_1dblpt_sup0_inf30.xlsx
+++ b/dossiers/stats_corpus_1dblpt_sup0_inf30.xlsx
@@ -8,30 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\dossiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A85FF6-14D6-48C8-8904-23B13D1BD91B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F842B3-5EAB-40B9-AF2A-86F9EBD26D98}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TYPE" sheetId="1" r:id="rId1"/>
     <sheet name="YEAR" sheetId="2" r:id="rId2"/>
     <sheet name="LENGTH" sheetId="3" r:id="rId3"/>
     <sheet name="LENGTH Méd" sheetId="11" r:id="rId4"/>
-    <sheet name="Count after dblpt" sheetId="12" r:id="rId5"/>
-    <sheet name="DOMAIN" sheetId="4" r:id="rId6"/>
-    <sheet name="AUTHORS" sheetId="5" r:id="rId7"/>
-    <sheet name="SPECIALS" sheetId="6" r:id="rId8"/>
-    <sheet name="SENTENCE" sheetId="7" r:id="rId9"/>
-    <sheet name="SEGMENTATION" sheetId="8" r:id="rId10"/>
-    <sheet name="AUTHORS LENGTH" sheetId="9" r:id="rId11"/>
-    <sheet name="SENTENCE DOMAIN" sheetId="10" r:id="rId12"/>
+    <sheet name="LENGTH OK" sheetId="13" r:id="rId5"/>
+    <sheet name="Count after dblpt" sheetId="12" r:id="rId6"/>
+    <sheet name="DOMAIN" sheetId="4" r:id="rId7"/>
+    <sheet name="AUTHORS" sheetId="5" r:id="rId8"/>
+    <sheet name="SPECIALS" sheetId="6" r:id="rId9"/>
+    <sheet name="SENTENCE" sheetId="7" r:id="rId10"/>
+    <sheet name="SEGMENTATION" sheetId="8" r:id="rId11"/>
+    <sheet name="AUTHORS LENGTH" sheetId="9" r:id="rId12"/>
+    <sheet name="SENTENCE DOMAIN" sheetId="10" r:id="rId13"/>
   </sheets>
   <calcPr calcId="179017"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="120">
   <si>
     <t>VIDEO</t>
   </si>
@@ -383,12 +391,21 @@
   <si>
     <t>MAX</t>
   </si>
+  <si>
+    <t>ATTENTION !</t>
+  </si>
+  <si>
+    <t>COMPTE FAIT AVEC LA PONCTUATION !</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,8 +428,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -428,6 +452,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,7 +607,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -610,6 +640,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1307,6 +1344,35 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1">
+        <v>6710</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2">
+        <v>78821</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -1447,7 +1513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C760"/>
   <sheetViews>
@@ -9820,7 +9886,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -10949,15 +11015,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>111</v>
       </c>
@@ -10974,7 +11040,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>15</v>
       </c>
@@ -10994,7 +11060,7 @@
         <v>82950</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>16</v>
       </c>
@@ -11014,7 +11080,7 @@
         <v>86112</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>14</v>
       </c>
@@ -11033,8 +11099,14 @@
         <f t="shared" si="1"/>
         <v>75138</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>17</v>
       </c>
@@ -11053,8 +11125,14 @@
         <f t="shared" si="1"/>
         <v>87686</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>13</v>
       </c>
@@ -11074,7 +11152,7 @@
         <v>66729</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>12</v>
       </c>
@@ -11094,7 +11172,7 @@
         <v>59460</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>18</v>
       </c>
@@ -11114,7 +11192,7 @@
         <v>88074</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>11</v>
       </c>
@@ -11134,7 +11212,7 @@
         <v>48840</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>19</v>
       </c>
@@ -11154,7 +11232,7 @@
         <v>83790</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20</v>
       </c>
@@ -11174,7 +11252,7 @@
         <v>79660</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -11194,7 +11272,7 @@
         <v>37150</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>21</v>
       </c>
@@ -11214,7 +11292,7 @@
         <v>76062</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>22</v>
       </c>
@@ -11234,7 +11312,7 @@
         <v>68552</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>23</v>
       </c>
@@ -11254,7 +11332,7 @@
         <v>65665</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9</v>
       </c>
@@ -11914,7 +11992,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>51</v>
       </c>
@@ -11934,7 +12012,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>52</v>
       </c>
@@ -11954,7 +12032,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -11974,7 +12052,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>53</v>
       </c>
@@ -11994,7 +12072,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>54</v>
       </c>
@@ -12014,7 +12092,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>57</v>
       </c>
@@ -12034,7 +12112,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>55</v>
       </c>
@@ -12054,7 +12132,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>58</v>
       </c>
@@ -12074,7 +12152,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>62</v>
       </c>
@@ -12094,7 +12172,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>64</v>
       </c>
@@ -12114,7 +12192,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>59</v>
       </c>
@@ -12134,7 +12212,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>63</v>
       </c>
@@ -12154,7 +12232,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>56</v>
       </c>
@@ -12173,8 +12251,14 @@
         <f t="shared" si="1"/>
         <v>336</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H61" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="I61" s="33"/>
+      <c r="J61" s="33"/>
+      <c r="K61" s="33"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>68</v>
       </c>
@@ -12193,8 +12277,14 @@
         <f t="shared" si="1"/>
         <v>340</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H62" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="I62" s="33"/>
+      <c r="J62" s="33"/>
+      <c r="K62" s="33"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>67</v>
       </c>
@@ -12214,7 +12304,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>65</v>
       </c>
@@ -12699,16 +12789,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H86"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>111</v>
       </c>
@@ -12723,7 +12813,7 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -12739,7 +12829,7 @@
         <v>3.7413335515777907E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -12755,7 +12845,7 @@
         <v>1.2276250716114624E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -12771,7 +12861,7 @@
         <v>4.3142252516631396E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -12786,8 +12876,14 @@
         <f t="shared" si="1"/>
         <v>1.1937192363002887E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
@@ -12802,8 +12898,14 @@
         <f t="shared" si="1"/>
         <v>2.6960984906057452E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8</v>
       </c>
@@ -12819,7 +12921,7 @@
         <v>5.1010744642293437E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
@@ -12835,7 +12937,7 @@
         <v>8.4378763255427855E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10</v>
       </c>
@@ -12851,7 +12953,7 @@
         <v>0.12781330745577626</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11</v>
       </c>
@@ -12867,7 +12969,7 @@
         <v>0.1797243104839181</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>12</v>
       </c>
@@ -12883,7 +12985,7 @@
         <v>0.23765652219663044</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>13</v>
       </c>
@@ -12899,7 +13001,7 @@
         <v>0.29766985069740792</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>14</v>
       </c>
@@ -12915,7 +13017,7 @@
         <v>0.3604190293577767</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>15</v>
       </c>
@@ -12931,7 +13033,7 @@
         <v>0.4250739497959804</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>16</v>
       </c>
@@ -12947,7 +13049,7 @@
         <v>0.48799850346657936</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>17</v>
       </c>
@@ -13767,7 +13869,7 @@
         <v>5</v>
       </c>
       <c r="C66" s="1">
-        <f t="shared" ref="C66:C97" si="3">B66/85531</f>
+        <f t="shared" ref="C66:C85" si="3">B66/85531</f>
         <v>5.845833674340298E-5</v>
       </c>
       <c r="D66" s="2">
@@ -14091,11 +14193,1375 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5819BF2F-AE87-4467-82FC-8C0357A2C619}">
+  <dimension ref="A1:K66"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="9.140625" style="31"/>
+    <col min="5" max="5" width="9.140625" style="34"/>
+    <col min="6" max="16384" width="9.140625" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="31">
+        <v>2</v>
+      </c>
+      <c r="B1" s="31">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1">
+        <f>B1/85531</f>
+        <v>3.9751668985514024E-4</v>
+      </c>
+      <c r="E1" s="34">
+        <f>D1</f>
+        <v>3.9751668985514024E-4</v>
+      </c>
+      <c r="H1" s="31">
+        <f>B1*A1</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="31">
+        <v>3</v>
+      </c>
+      <c r="B2" s="31">
+        <v>103</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:D65" si="0">B2/85531</f>
+        <v>1.2042417369141013E-3</v>
+      </c>
+      <c r="E2" s="34">
+        <f>D2+E1</f>
+        <v>1.6017584267692415E-3</v>
+      </c>
+      <c r="H2" s="31">
+        <f t="shared" ref="H2:H65" si="1">B2*A2</f>
+        <v>309</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="31">
+        <v>4</v>
+      </c>
+      <c r="B3" s="31">
+        <v>392</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="35">
+        <f t="shared" si="0"/>
+        <v>4.5831336006827931E-3</v>
+      </c>
+      <c r="E3" s="36">
+        <f t="shared" ref="E3:E66" si="2">D3+E2</f>
+        <v>6.1848920274520346E-3</v>
+      </c>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32">
+        <f t="shared" si="1"/>
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="31">
+        <v>5</v>
+      </c>
+      <c r="B4" s="31">
+        <v>900</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="35">
+        <f t="shared" si="0"/>
+        <v>1.0522500613812536E-2</v>
+      </c>
+      <c r="E4" s="36">
+        <f t="shared" si="2"/>
+        <v>1.6707392641264571E-2</v>
+      </c>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32">
+        <f t="shared" si="1"/>
+        <v>4500</v>
+      </c>
+      <c r="K4" s="37"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="31">
+        <v>6</v>
+      </c>
+      <c r="B5" s="31">
+        <v>1794</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" s="35">
+        <f t="shared" si="0"/>
+        <v>2.0974851223532986E-2</v>
+      </c>
+      <c r="E5" s="36">
+        <f t="shared" si="2"/>
+        <v>3.7682243864797557E-2</v>
+      </c>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32">
+        <f t="shared" si="1"/>
+        <v>10764</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="31">
+        <v>7</v>
+      </c>
+      <c r="B6" s="31">
+        <v>2597</v>
+      </c>
+      <c r="C6" s="32"/>
+      <c r="D6" s="35">
+        <f t="shared" si="0"/>
+        <v>3.0363260104523507E-2</v>
+      </c>
+      <c r="E6" s="36">
+        <f t="shared" si="2"/>
+        <v>6.8045503969321061E-2</v>
+      </c>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32">
+        <f t="shared" si="1"/>
+        <v>18179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
+        <v>8</v>
+      </c>
+      <c r="B7" s="31">
+        <v>3579</v>
+      </c>
+      <c r="C7" s="32"/>
+      <c r="D7" s="35">
+        <f t="shared" si="0"/>
+        <v>4.1844477440927848E-2</v>
+      </c>
+      <c r="E7" s="36">
+        <f t="shared" si="2"/>
+        <v>0.10988998141024892</v>
+      </c>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32">
+        <f t="shared" si="1"/>
+        <v>28632</v>
+      </c>
+      <c r="K7" s="37"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
+        <v>9</v>
+      </c>
+      <c r="B8" s="31">
+        <v>4439</v>
+      </c>
+      <c r="C8" s="32"/>
+      <c r="D8" s="35">
+        <f t="shared" si="0"/>
+        <v>5.1899311360793163E-2</v>
+      </c>
+      <c r="E8" s="36">
+        <f t="shared" si="2"/>
+        <v>0.16178929277104209</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32">
+        <f t="shared" si="1"/>
+        <v>39951</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="20">
+        <v>10</v>
+      </c>
+      <c r="B9" s="20">
+        <v>5110</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21">
+        <f t="shared" si="0"/>
+        <v>5.9744420151757842E-2</v>
+      </c>
+      <c r="E9" s="38">
+        <f t="shared" si="2"/>
+        <v>0.22153371292279994</v>
+      </c>
+      <c r="H9" s="31">
+        <f t="shared" si="1"/>
+        <v>51100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="20">
+        <v>11</v>
+      </c>
+      <c r="B10" s="20">
+        <v>5539</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21">
+        <f t="shared" si="0"/>
+        <v>6.4760145444341818E-2</v>
+      </c>
+      <c r="E10" s="38">
+        <f t="shared" si="2"/>
+        <v>0.28629385836714177</v>
+      </c>
+      <c r="H10" s="31">
+        <f t="shared" si="1"/>
+        <v>60929</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="32">
+        <v>12</v>
+      </c>
+      <c r="B11" s="32">
+        <v>5654</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>6.6104687189440084E-2</v>
+      </c>
+      <c r="E11" s="34">
+        <f t="shared" si="2"/>
+        <v>0.35239854555658184</v>
+      </c>
+      <c r="H11" s="31">
+        <f t="shared" si="1"/>
+        <v>67848</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="31">
+        <v>13</v>
+      </c>
+      <c r="B12" s="31">
+        <v>5965</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>6.9740795734879749E-2</v>
+      </c>
+      <c r="E12" s="34">
+        <f t="shared" si="2"/>
+        <v>0.42213934129146158</v>
+      </c>
+      <c r="H12" s="31">
+        <f t="shared" si="1"/>
+        <v>77545</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
+        <v>14</v>
+      </c>
+      <c r="B13" s="20">
+        <v>5764</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21">
+        <f t="shared" si="0"/>
+        <v>6.7390770597794955E-2</v>
+      </c>
+      <c r="E13" s="38">
+        <f t="shared" si="2"/>
+        <v>0.48953011188925655</v>
+      </c>
+      <c r="H13" s="31">
+        <f t="shared" si="1"/>
+        <v>80696</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="20">
+        <v>15</v>
+      </c>
+      <c r="B14" s="20">
+        <v>5666</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21">
+        <f t="shared" si="0"/>
+        <v>6.6244987197624255E-2</v>
+      </c>
+      <c r="E14" s="38">
+        <f t="shared" si="2"/>
+        <v>0.55577509908688083</v>
+      </c>
+      <c r="H14" s="31">
+        <f t="shared" si="1"/>
+        <v>84990</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="32">
+        <v>16</v>
+      </c>
+      <c r="B15" s="32">
+        <v>5203</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>6.083174521518514E-2</v>
+      </c>
+      <c r="E15" s="34">
+        <f t="shared" si="2"/>
+        <v>0.61660684430206603</v>
+      </c>
+      <c r="H15" s="31">
+        <f t="shared" si="1"/>
+        <v>83248</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="32">
+        <v>17</v>
+      </c>
+      <c r="B16" s="32">
+        <v>4774</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>5.5816019922601164E-2</v>
+      </c>
+      <c r="E16" s="34">
+        <f t="shared" si="2"/>
+        <v>0.67242286422466724</v>
+      </c>
+      <c r="H16" s="31">
+        <f t="shared" si="1"/>
+        <v>81158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="31">
+        <v>18</v>
+      </c>
+      <c r="B17" s="31">
+        <v>4274</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>4.9970186248260863E-2</v>
+      </c>
+      <c r="E17" s="34">
+        <f t="shared" si="2"/>
+        <v>0.72239305047292812</v>
+      </c>
+      <c r="H17" s="31">
+        <f t="shared" si="1"/>
+        <v>76932</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="31">
+        <v>19</v>
+      </c>
+      <c r="B18" s="31">
+        <v>3853</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>4.5047994294466334E-2</v>
+      </c>
+      <c r="E18" s="34">
+        <f t="shared" si="2"/>
+        <v>0.7674410447673945</v>
+      </c>
+      <c r="H18" s="31">
+        <f t="shared" si="1"/>
+        <v>73207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="31">
+        <v>20</v>
+      </c>
+      <c r="B19" s="31">
+        <v>3327</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>3.8898177269060343E-2</v>
+      </c>
+      <c r="E19" s="34">
+        <f t="shared" si="2"/>
+        <v>0.80633922203645481</v>
+      </c>
+      <c r="H19" s="31">
+        <f t="shared" si="1"/>
+        <v>66540</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="31">
+        <v>21</v>
+      </c>
+      <c r="B20" s="31">
+        <v>2819</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2958810255930601E-2</v>
+      </c>
+      <c r="E20" s="34">
+        <f t="shared" si="2"/>
+        <v>0.83929803229238542</v>
+      </c>
+      <c r="H20" s="31">
+        <f t="shared" si="1"/>
+        <v>59199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="31">
+        <v>22</v>
+      </c>
+      <c r="B21" s="31">
+        <v>2433</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8445826659339889E-2</v>
+      </c>
+      <c r="E21" s="34">
+        <f t="shared" si="2"/>
+        <v>0.86774385895172534</v>
+      </c>
+      <c r="H21" s="31">
+        <f t="shared" si="1"/>
+        <v>53526</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="31">
+        <v>23</v>
+      </c>
+      <c r="B22" s="31">
+        <v>2042</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3874384726005775E-2</v>
+      </c>
+      <c r="E22" s="34">
+        <f t="shared" si="2"/>
+        <v>0.89161824367773113</v>
+      </c>
+      <c r="H22" s="31">
+        <f t="shared" si="1"/>
+        <v>46966</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="31">
+        <v>24</v>
+      </c>
+      <c r="B23" s="31">
+        <v>1660</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>1.940816779880979E-2</v>
+      </c>
+      <c r="E23" s="34">
+        <f t="shared" si="2"/>
+        <v>0.91102641147654095</v>
+      </c>
+      <c r="H23" s="31">
+        <f t="shared" si="1"/>
+        <v>39840</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="31">
+        <v>25</v>
+      </c>
+      <c r="B24" s="31">
+        <v>1433</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6754159310659295E-2</v>
+      </c>
+      <c r="E24" s="34">
+        <f t="shared" si="2"/>
+        <v>0.92778057078720022</v>
+      </c>
+      <c r="H24" s="31">
+        <f t="shared" si="1"/>
+        <v>35825</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="31">
+        <v>26</v>
+      </c>
+      <c r="B25" s="31">
+        <v>1189</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3901392477581228E-2</v>
+      </c>
+      <c r="E25" s="34">
+        <f t="shared" si="2"/>
+        <v>0.94168196326478149</v>
+      </c>
+      <c r="H25" s="31">
+        <f t="shared" si="1"/>
+        <v>30914</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="31">
+        <v>27</v>
+      </c>
+      <c r="B26" s="31">
+        <v>946</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1060317311851843E-2</v>
+      </c>
+      <c r="E26" s="34">
+        <f t="shared" si="2"/>
+        <v>0.95274228057663335</v>
+      </c>
+      <c r="H26" s="31">
+        <f t="shared" si="1"/>
+        <v>25542</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="31">
+        <v>28</v>
+      </c>
+      <c r="B27" s="31">
+        <v>770</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>9.0025838584840579E-3</v>
+      </c>
+      <c r="E27" s="34">
+        <f t="shared" si="2"/>
+        <v>0.96174486443511742</v>
+      </c>
+      <c r="H27" s="31">
+        <f t="shared" si="1"/>
+        <v>21560</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="31">
+        <v>29</v>
+      </c>
+      <c r="B28" s="31">
+        <v>670</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>7.8334171236159982E-3</v>
+      </c>
+      <c r="E28" s="34">
+        <f t="shared" si="2"/>
+        <v>0.96957828155873338</v>
+      </c>
+      <c r="H28" s="31">
+        <f t="shared" si="1"/>
+        <v>19430</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="31">
+        <v>30</v>
+      </c>
+      <c r="B29" s="31">
+        <v>487</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
+        <v>5.6938419988074498E-3</v>
+      </c>
+      <c r="E29" s="34">
+        <f t="shared" si="2"/>
+        <v>0.97527212355754078</v>
+      </c>
+      <c r="H29" s="31">
+        <f t="shared" si="1"/>
+        <v>14610</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="31">
+        <v>31</v>
+      </c>
+      <c r="B30" s="31">
+        <v>427</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="0"/>
+        <v>4.9923419578866146E-3</v>
+      </c>
+      <c r="E30" s="34">
+        <f t="shared" si="2"/>
+        <v>0.98026446551542734</v>
+      </c>
+      <c r="H30" s="31">
+        <f t="shared" si="1"/>
+        <v>13237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="31">
+        <v>32</v>
+      </c>
+      <c r="B31" s="31">
+        <v>371</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>4.3376085863605007E-3</v>
+      </c>
+      <c r="E31" s="34">
+        <f t="shared" si="2"/>
+        <v>0.98460207410178779</v>
+      </c>
+      <c r="H31" s="31">
+        <f t="shared" si="1"/>
+        <v>11872</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="31">
+        <v>33</v>
+      </c>
+      <c r="B32" s="31">
+        <v>265</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>3.0982918474003578E-3</v>
+      </c>
+      <c r="E32" s="34">
+        <f t="shared" si="2"/>
+        <v>0.9877003659491882</v>
+      </c>
+      <c r="H32" s="31">
+        <f t="shared" si="1"/>
+        <v>8745</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="31">
+        <v>34</v>
+      </c>
+      <c r="B33" s="31">
+        <v>220</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="0"/>
+        <v>2.572166816709731E-3</v>
+      </c>
+      <c r="E33" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99027253276589788</v>
+      </c>
+      <c r="H33" s="31">
+        <f t="shared" si="1"/>
+        <v>7480</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="31">
+        <v>35</v>
+      </c>
+      <c r="B34" s="31">
+        <v>155</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8122084390454923E-3</v>
+      </c>
+      <c r="E34" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99208474120494339</v>
+      </c>
+      <c r="H34" s="31">
+        <f t="shared" si="1"/>
+        <v>5425</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="31">
+        <v>36</v>
+      </c>
+      <c r="B35" s="31">
+        <v>139</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6251417614666027E-3</v>
+      </c>
+      <c r="E35" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99370988296640994</v>
+      </c>
+      <c r="H35" s="31">
+        <f t="shared" si="1"/>
+        <v>5004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="31">
+        <v>37</v>
+      </c>
+      <c r="B36" s="31">
+        <v>100</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1691667348680595E-3</v>
+      </c>
+      <c r="E36" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99487904970127805</v>
+      </c>
+      <c r="H36" s="31">
+        <f t="shared" si="1"/>
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="31">
+        <v>38</v>
+      </c>
+      <c r="B37" s="31">
+        <v>82</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="0"/>
+        <v>9.5871672259180884E-4</v>
+      </c>
+      <c r="E37" s="34">
+        <f t="shared" si="2"/>
+        <v>0.9958377664238699</v>
+      </c>
+      <c r="H37" s="31">
+        <f t="shared" si="1"/>
+        <v>3116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="31">
+        <v>39</v>
+      </c>
+      <c r="B38" s="31">
+        <v>82</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="0"/>
+        <v>9.5871672259180884E-4</v>
+      </c>
+      <c r="E38" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99679648314646174</v>
+      </c>
+      <c r="H38" s="31">
+        <f t="shared" si="1"/>
+        <v>3198</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="31">
+        <v>40</v>
+      </c>
+      <c r="B39" s="31">
+        <v>47</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4950836538798797E-4</v>
+      </c>
+      <c r="E39" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99734599151184977</v>
+      </c>
+      <c r="H39" s="31">
+        <f t="shared" si="1"/>
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="31">
+        <v>41</v>
+      </c>
+      <c r="B40" s="31">
+        <v>43</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="0"/>
+        <v>5.0274169599326564E-4</v>
+      </c>
+      <c r="E40" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99784873320784306</v>
+      </c>
+      <c r="H40" s="31">
+        <f t="shared" si="1"/>
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="31">
+        <v>42</v>
+      </c>
+      <c r="B41" s="31">
+        <v>28</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2736668576305669E-4</v>
+      </c>
+      <c r="E41" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99817609989360612</v>
+      </c>
+      <c r="H41" s="31">
+        <f t="shared" si="1"/>
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="31">
+        <v>43</v>
+      </c>
+      <c r="B42" s="31">
+        <v>29</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3905835311173727E-4</v>
+      </c>
+      <c r="E42" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99851515824671788</v>
+      </c>
+      <c r="H42" s="31">
+        <f t="shared" si="1"/>
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="31">
+        <v>44</v>
+      </c>
+      <c r="B43" s="31">
+        <v>22</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5721668167097308E-4</v>
+      </c>
+      <c r="E43" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99877237492838888</v>
+      </c>
+      <c r="H43" s="31">
+        <f t="shared" si="1"/>
+        <v>968</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="31">
+        <v>45</v>
+      </c>
+      <c r="B44" s="31">
+        <v>21</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="0"/>
+        <v>2.455250143222925E-4</v>
+      </c>
+      <c r="E44" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99901789994271117</v>
+      </c>
+      <c r="H44" s="31">
+        <f t="shared" si="1"/>
+        <v>945</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="31">
+        <v>46</v>
+      </c>
+      <c r="B45" s="31">
+        <v>9</v>
+      </c>
+      <c r="D45" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0522500613812536E-4</v>
+      </c>
+      <c r="E45" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99912312494884925</v>
+      </c>
+      <c r="H45" s="31">
+        <f t="shared" si="1"/>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="31">
+        <v>47</v>
+      </c>
+      <c r="B46" s="31">
+        <v>15</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7537501023020893E-4</v>
+      </c>
+      <c r="E46" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99929849995907949</v>
+      </c>
+      <c r="H46" s="31">
+        <f t="shared" si="1"/>
+        <v>705</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="31">
+        <v>48</v>
+      </c>
+      <c r="B47" s="31">
+        <v>8</v>
+      </c>
+      <c r="D47" s="1">
+        <f t="shared" si="0"/>
+        <v>9.3533338789444768E-5</v>
+      </c>
+      <c r="E47" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99939203329786896</v>
+      </c>
+      <c r="H47" s="31">
+        <f t="shared" si="1"/>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="31">
+        <v>49</v>
+      </c>
+      <c r="B48" s="31">
+        <v>12</v>
+      </c>
+      <c r="D48" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4030000818416715E-4</v>
+      </c>
+      <c r="E48" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99953233330605318</v>
+      </c>
+      <c r="H48" s="31">
+        <f t="shared" si="1"/>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="31">
+        <v>50</v>
+      </c>
+      <c r="B49" s="31">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3383334697361192E-5</v>
+      </c>
+      <c r="E49" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99955571664075049</v>
+      </c>
+      <c r="H49" s="31">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="31">
+        <v>51</v>
+      </c>
+      <c r="B50" s="31">
+        <v>6</v>
+      </c>
+      <c r="D50" s="1">
+        <f t="shared" si="0"/>
+        <v>7.0150004092083576E-5</v>
+      </c>
+      <c r="E50" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99962586664484254</v>
+      </c>
+      <c r="H50" s="31">
+        <f t="shared" si="1"/>
+        <v>306</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="31">
+        <v>52</v>
+      </c>
+      <c r="B51" s="31">
+        <v>2</v>
+      </c>
+      <c r="D51" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3383334697361192E-5</v>
+      </c>
+      <c r="E51" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99964924997953986</v>
+      </c>
+      <c r="H51" s="31">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="31">
+        <v>53</v>
+      </c>
+      <c r="B52" s="31">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3383334697361192E-5</v>
+      </c>
+      <c r="E52" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99967263331423717</v>
+      </c>
+      <c r="H52" s="31">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="31">
+        <v>54</v>
+      </c>
+      <c r="B53" s="31">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3383334697361192E-5</v>
+      </c>
+      <c r="E53" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99969601664893448</v>
+      </c>
+      <c r="H53" s="31">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="31">
+        <v>55</v>
+      </c>
+      <c r="B54" s="31">
+        <v>5</v>
+      </c>
+      <c r="D54" s="1">
+        <f t="shared" si="0"/>
+        <v>5.845833674340298E-5</v>
+      </c>
+      <c r="E54" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99975447498567793</v>
+      </c>
+      <c r="H54" s="31">
+        <f t="shared" si="1"/>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="31">
+        <v>56</v>
+      </c>
+      <c r="B55" s="31">
+        <v>2</v>
+      </c>
+      <c r="D55" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3383334697361192E-5</v>
+      </c>
+      <c r="E55" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99977785832037525</v>
+      </c>
+      <c r="H55" s="31">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="31">
+        <v>57</v>
+      </c>
+      <c r="B56" s="31">
+        <v>6</v>
+      </c>
+      <c r="D56" s="1">
+        <f t="shared" si="0"/>
+        <v>7.0150004092083576E-5</v>
+      </c>
+      <c r="E56" s="34">
+        <f t="shared" si="2"/>
+        <v>0.9998480083244673</v>
+      </c>
+      <c r="H56" s="31">
+        <f t="shared" si="1"/>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="31">
+        <v>58</v>
+      </c>
+      <c r="B57" s="31">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1691667348680596E-5</v>
+      </c>
+      <c r="E57" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99985969999181601</v>
+      </c>
+      <c r="H57" s="31">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="31">
+        <v>59</v>
+      </c>
+      <c r="B58" s="31">
+        <v>1</v>
+      </c>
+      <c r="D58" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1691667348680596E-5</v>
+      </c>
+      <c r="E58" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99987139165916472</v>
+      </c>
+      <c r="H58" s="31">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="31">
+        <v>60</v>
+      </c>
+      <c r="B59" s="31">
+        <v>2</v>
+      </c>
+      <c r="D59" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3383334697361192E-5</v>
+      </c>
+      <c r="E59" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99989477499386203</v>
+      </c>
+      <c r="H59" s="31">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="31">
+        <v>61</v>
+      </c>
+      <c r="B60" s="31">
+        <v>2</v>
+      </c>
+      <c r="D60" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3383334697361192E-5</v>
+      </c>
+      <c r="E60" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99991815832855935</v>
+      </c>
+      <c r="H60" s="31">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="31">
+        <v>63</v>
+      </c>
+      <c r="B61" s="31">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1691667348680596E-5</v>
+      </c>
+      <c r="E61" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99992984999590806</v>
+      </c>
+      <c r="H61" s="31">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="31">
+        <v>64</v>
+      </c>
+      <c r="B62" s="31">
+        <v>2</v>
+      </c>
+      <c r="D62" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3383334697361192E-5</v>
+      </c>
+      <c r="E62" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99995323333060537</v>
+      </c>
+      <c r="H62" s="31">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="31">
+        <v>66</v>
+      </c>
+      <c r="B63" s="31">
+        <v>1</v>
+      </c>
+      <c r="D63" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1691667348680596E-5</v>
+      </c>
+      <c r="E63" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99996492499795409</v>
+      </c>
+      <c r="H63" s="31">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="31">
+        <v>67</v>
+      </c>
+      <c r="B64" s="31">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1691667348680596E-5</v>
+      </c>
+      <c r="E64" s="34">
+        <f t="shared" si="2"/>
+        <v>0.9999766166653028</v>
+      </c>
+      <c r="H64" s="31">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="31">
+        <v>68</v>
+      </c>
+      <c r="B65" s="31">
+        <v>1</v>
+      </c>
+      <c r="D65" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1691667348680596E-5</v>
+      </c>
+      <c r="E65" s="34">
+        <f t="shared" si="2"/>
+        <v>0.99998830833265151</v>
+      </c>
+      <c r="H65" s="31">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="31">
+        <v>69</v>
+      </c>
+      <c r="B66" s="31">
+        <v>1</v>
+      </c>
+      <c r="D66" s="1">
+        <f t="shared" ref="D66" si="3">B66/85531</f>
+        <v>1.1691667348680596E-5</v>
+      </c>
+      <c r="E66" s="34">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="H66" s="31">
+        <f t="shared" ref="H66" si="4">B66*A66</f>
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7261A088-0697-451E-9BB3-F775B6F58077}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14430,7 +15896,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -14558,7 +16024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
@@ -15339,28 +16805,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B1">
-        <v>3508</v>
+        <v>85531</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="B2">
-        <v>3493</v>
+        <v>9609</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -15373,26 +16841,26 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B4">
-        <v>341</v>
+        <v>3708</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B5">
-        <v>85531</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6">
-        <v>3708</v>
+        <v>3508</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="31">
+        <v>3493</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -15403,36 +16871,18 @@
         <v>360</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8">
+        <v>341</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1">
-        <v>6710</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2">
-        <v>78821</v>
-      </c>
-    </row>
-  </sheetData>
+  <sortState ref="A1:B8">
+    <sortCondition descending="1" ref="B1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>